<commit_message>
actualización bodega, convenior, ecommerce, excluidos, exhibiciones
</commit_message>
<xml_diff>
--- a/data/input/excluidos/codigos_excluidos.xlsx
+++ b/data/input/excluidos/codigos_excluidos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\desarrollo\promedios-ventas-pdv\data\input\excluidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\desarrollo\gestionCompras\data\input\excluidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD668E8D-085A-4AE6-9985-9AE371D3324A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7580CBCD-2ECB-438D-B60E-13261F4FD0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EBD8057D-B17E-478F-AC81-CD15BB3C498E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EBD8057D-B17E-478F-AC81-CD15BB3C498E}"/>
   </bookViews>
   <sheets>
     <sheet name="codigos_excluidos" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>codigo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>TOTALGENERAL</t>
   </si>
@@ -51,6 +45,9 @@
   </si>
   <si>
     <t>TOTAL GENERAL</t>
+  </si>
+  <si>
+    <t>Codigo</t>
   </si>
 </sst>
 </file>
@@ -534,8 +531,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -922,587 +920,374 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FC1072-E46D-4D2E-80F4-FC5232F14ABE}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:A71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>500000292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>94412029</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>16685167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>500000292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1143840869</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1130654230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1105682139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16537078</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>500000294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>94544009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1110363405</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1110362459</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1143937287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>460223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>770016720</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>770016047</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>770015835</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>770013910</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>770013591</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>770013770</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>770015832</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>770017556</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>94429938</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>500000293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>79607131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>79601131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>500000289</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>124569</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>139003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>770019213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>770018167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>770018289</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>770014422</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>770016589</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>770013809</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>770014278</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>770013435</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>770012656</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>770011350</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>770017266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>770018662</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>770018981</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>770014351</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>770017052</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>770014561</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>770018465</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>770010462</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>770007391</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>770005931</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>770007620</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>770002952</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>770005952</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>770005997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>500000132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>105323</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>700105323</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>500000133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>105329</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>700105329</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>105332</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>700105332</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>105333</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>700105333</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>94412029</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>16685167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1143840869</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>1130654230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1105682139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>16537078</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>500000294</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>94544009</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>1110363405</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>1110362459</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>1143937287</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>460223</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>770016720</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>770016047</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>770015835</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>770013910</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>770013591</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>770013770</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>770015832</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>770017556</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>94429938</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>500000293</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>79607131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>79601131</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>500000289</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>124569</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>139003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>770019213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>770018167</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>770018289</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>770014422</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>770016589</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>770013809</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>770014278</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>770013435</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>770012656</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>770011350</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>770017266</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>770018662</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>770018981</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>770014351</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49">
-        <v>770017052</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>770014561</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <v>770018465</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <v>770010462</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <v>770007391</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54">
-        <v>770005931</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55">
-        <v>770007620</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <v>770002952</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <v>770005952</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <v>770005997</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>500000132</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>105323</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>700105323</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>500000133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>105329</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64">
-        <v>700105329</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <v>105332</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66">
-        <v>700105332</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67">
-        <v>105333</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68">
-        <v>700105333</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70">
         <v>94531361</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71">
         <v>1113621290</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactor ETL runners to include loaders for various data types
- Added loaders for 'excluidos', 'exhibiciones', 'gerencia', 'inactivos', 'inventario', 'maestra_inventario', 'merchandising', 'mostrador', 'oferta', 'quincenales', 'semanales', 'temporales', 'transferencias', and 'ventas'.
- Updated the key generation functions to prefix with 'stg_' for consistency.
- Modified the directory paths for 'inactivos' and 'maestra_inventario' to use underscores instead of hyphens.
- Enhanced the transform functions to handle data processing more robustly.
- Implemented a base loader class to streamline the loading process into the database.
- Removed unnecessary comments and improved code readability.
- Added new loader classes for 'convenios', 'correos_laboratorios', and 'ecommerce'.
</commit_message>
<xml_diff>
--- a/data/input/excluidos/codigos_excluidos.xlsx
+++ b/data/input/excluidos/codigos_excluidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\desarrollo\gestionCompras\data\input\excluidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7580CBCD-2ECB-438D-B60E-13261F4FD0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C269E47-B3A4-4CBE-A1AE-70249BC2C862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EBD8057D-B17E-478F-AC81-CD15BB3C498E}"/>
   </bookViews>
@@ -531,9 +531,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -922,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FC1072-E46D-4D2E-80F4-FC5232F14ABE}">
   <dimension ref="A1:A71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +931,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>